<commit_message>
Add Notidicarion + Add Updating Price
</commit_message>
<xml_diff>
--- a/Bazaraki.xlsx
+++ b/Bazaraki.xlsx
@@ -34,18 +34,18 @@
     <t>Дата создания объявления</t>
   </si>
   <si>
+    <t>Shop in leoforos omonoias limassol</t>
+  </si>
+  <si>
+    <t>https://www.bazaraki.com/adv/4721374_shop-in-leoforos-omonoias/</t>
+  </si>
+  <si>
     <t>Exceptional office space in limassol center</t>
   </si>
   <si>
     <t>https://www.bazaraki.com/adv/4717864_exceptional-office-space-in-limassol-center/</t>
   </si>
   <si>
-    <t>Γραφειο στο κέντρο της πολης</t>
-  </si>
-  <si>
-    <t>https://www.bazaraki.com/adv/4717648_grapheio-sto-kentro-tes-poles/</t>
-  </si>
-  <si>
     <t>Office in agias zonis area</t>
   </si>
   <si>
@@ -88,12 +88,6 @@
     <t>https://www.bazaraki.com/adv/4707466_shop-in-limassol-cyprus/</t>
   </si>
   <si>
-    <t>Shop, retail, central location</t>
-  </si>
-  <si>
-    <t>https://www.bazaraki.com/adv/4707211_shop-retail-central-location/</t>
-  </si>
-  <si>
     <t>Office, near new port</t>
   </si>
   <si>
@@ -295,12 +289,6 @@
     <t>https://www.bazaraki.com/adv/4652937_commercial-office-in-katholiki-limassol/</t>
   </si>
   <si>
-    <t>120m office space in kato polemidia, limassol</t>
-  </si>
-  <si>
-    <t>https://www.bazaraki.com/adv/4646972_120m-office-space-in-kato-polemidia-limassol/</t>
-  </si>
-  <si>
     <t>231sqm office in agios athanasios</t>
   </si>
   <si>
@@ -403,7 +391,7 @@
     <t>https://www.bazaraki.com/adv/4558998_shop-a-at-agias-fylaxeos/</t>
   </si>
   <si>
-    <t>Famous restaurant</t>
+    <t>Ресторан - caffe с лицензией технического директора</t>
   </si>
   <si>
     <t>https://www.bazaraki.com/adv/4535313_restorant-in-tourist-area/</t>
@@ -695,6 +683,18 @@
   </si>
   <si>
     <t>https://www.bazaraki.com/adv/4169238_shop-in-germasogeia/</t>
+  </si>
+  <si>
+    <t>120sqm office in agios nikolaos, limassol</t>
+  </si>
+  <si>
+    <t>https://www.bazaraki.com/adv/4088917_120sqm-office-in-agios-nikolaos-limassol/</t>
+  </si>
+  <si>
+    <t>Commercial store in limassol centre</t>
+  </si>
+  <si>
+    <t>https://www.bazaraki.com/adv/3868167_commercial-store-in-limassol-centre/</t>
   </si>
 </sst>
 </file>
@@ -1029,7 +1029,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>4717864</v>
+        <v>4721374</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -1038,18 +1038,18 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>177</v>
+        <v>63</v>
       </c>
       <c r="E2">
-        <v>368000</v>
+        <v>120000</v>
       </c>
       <c r="F2" s="1">
-        <v>45068.51038194444</v>
+        <v>45070.55881944444</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>4717648</v>
+        <v>4717864</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -1058,13 +1058,13 @@
         <v>9</v>
       </c>
       <c r="D3">
-        <v>110</v>
+        <v>177</v>
       </c>
       <c r="E3">
-        <v>240000</v>
+        <v>368000</v>
       </c>
       <c r="F3" s="1">
-        <v>45068.432442129626</v>
+        <v>45068.51038194444</v>
       </c>
     </row>
     <row r="4">
@@ -1229,7 +1229,7 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>4707211</v>
+        <v>4707171</v>
       </c>
       <c r="B12" t="s">
         <v>24</v>
@@ -1238,18 +1238,18 @@
         <v>25</v>
       </c>
       <c r="D12">
-        <v>217</v>
+        <v>240</v>
       </c>
       <c r="E12">
-        <v>299000</v>
+        <v>370000</v>
       </c>
       <c r="F12" s="1">
-        <v>45062.64388888889</v>
+        <v>45062.64212962963</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>4707171</v>
+        <v>4707148</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
@@ -1258,18 +1258,18 @@
         <v>27</v>
       </c>
       <c r="D13">
-        <v>240</v>
+        <v>200</v>
       </c>
       <c r="E13">
-        <v>370000</v>
+        <v>550000</v>
       </c>
       <c r="F13" s="1">
-        <v>45062.64212962963</v>
+        <v>45062.640752314815</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>4707148</v>
+        <v>4704575</v>
       </c>
       <c r="B14" t="s">
         <v>28</v>
@@ -1278,18 +1278,18 @@
         <v>29</v>
       </c>
       <c r="D14">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="E14">
-        <v>550000</v>
+        <v>368000</v>
       </c>
       <c r="F14" s="1">
-        <v>45062.640752314815</v>
+        <v>45061.41887731481</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>4704575</v>
+        <v>4701709</v>
       </c>
       <c r="B15" t="s">
         <v>30</v>
@@ -1298,18 +1298,18 @@
         <v>31</v>
       </c>
       <c r="D15">
-        <v>177</v>
+        <v>141</v>
       </c>
       <c r="E15">
-        <v>368000</v>
+        <v>1600000</v>
       </c>
       <c r="F15" s="1">
-        <v>45061.41887731481</v>
+        <v>45058.62601851852</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>4701709</v>
+        <v>4701313</v>
       </c>
       <c r="B16" t="s">
         <v>32</v>
@@ -1318,18 +1318,18 @@
         <v>33</v>
       </c>
       <c r="D16">
-        <v>141</v>
+        <v>180</v>
       </c>
       <c r="E16">
-        <v>1600000</v>
+        <v>660000</v>
       </c>
       <c r="F16" s="1">
-        <v>45058.62601851852</v>
+        <v>45058.42391203704</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>4701313</v>
+        <v>4701114</v>
       </c>
       <c r="B17" t="s">
         <v>34</v>
@@ -1338,18 +1338,18 @@
         <v>35</v>
       </c>
       <c r="D17">
-        <v>180</v>
+        <v>205</v>
       </c>
       <c r="E17">
-        <v>660000</v>
+        <v>1600000</v>
       </c>
       <c r="F17" s="1">
-        <v>45058.42391203704</v>
+        <v>45058.37673611111</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>4701114</v>
+        <v>4700356</v>
       </c>
       <c r="B18" t="s">
         <v>36</v>
@@ -1358,18 +1358,18 @@
         <v>37</v>
       </c>
       <c r="D18">
-        <v>205</v>
+        <v>132</v>
       </c>
       <c r="E18">
-        <v>1600000</v>
+        <v>280000</v>
       </c>
       <c r="F18" s="1">
-        <v>45058.37673611111</v>
+        <v>45057.62741898148</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>4700356</v>
+        <v>4699442</v>
       </c>
       <c r="B19" t="s">
         <v>38</v>
@@ -1384,12 +1384,12 @@
         <v>280000</v>
       </c>
       <c r="F19" s="1">
-        <v>45057.62741898148</v>
+        <v>45057.377222222225</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>4699442</v>
+        <v>4699342</v>
       </c>
       <c r="B20" t="s">
         <v>40</v>
@@ -1398,18 +1398,18 @@
         <v>41</v>
       </c>
       <c r="D20">
-        <v>132</v>
+        <v>225</v>
       </c>
       <c r="E20">
-        <v>280000</v>
+        <v>500000</v>
       </c>
       <c r="F20" s="1">
-        <v>45057.377222222225</v>
+        <v>45057.33484953704</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>4699342</v>
+        <v>4698805</v>
       </c>
       <c r="B21" t="s">
         <v>42</v>
@@ -1418,58 +1418,58 @@
         <v>43</v>
       </c>
       <c r="D21">
-        <v>225</v>
+        <v>138</v>
       </c>
       <c r="E21">
-        <v>500000</v>
+        <v>850000</v>
       </c>
       <c r="F21" s="1">
-        <v>45057.33484953704</v>
+        <v>45056.751655092594</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>4698805</v>
+        <v>4698554</v>
       </c>
       <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
         <v>44</v>
-      </c>
-      <c r="C22" t="s">
-        <v>45</v>
       </c>
       <c r="D22">
         <v>138</v>
       </c>
       <c r="E22">
-        <v>850000</v>
+        <v>805000</v>
       </c>
       <c r="F22" s="1">
-        <v>45056.751655092594</v>
+        <v>45056.62635416666</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>4698554</v>
+        <v>4697055</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
         <v>46</v>
       </c>
       <c r="D23">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="E23">
-        <v>805000</v>
+        <v>300000</v>
       </c>
       <c r="F23" s="1">
-        <v>45056.62635416666</v>
+        <v>45055.605844907404</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>4697055</v>
+        <v>4696705</v>
       </c>
       <c r="B24" t="s">
         <v>47</v>
@@ -1478,18 +1478,18 @@
         <v>48</v>
       </c>
       <c r="D24">
-        <v>110</v>
+        <v>185</v>
       </c>
       <c r="E24">
-        <v>300000</v>
+        <v>540000</v>
       </c>
       <c r="F24" s="1">
-        <v>45055.605844907404</v>
+        <v>45055.50114583333</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>4696705</v>
+        <v>4696508</v>
       </c>
       <c r="B25" t="s">
         <v>49</v>
@@ -1498,18 +1498,18 @@
         <v>50</v>
       </c>
       <c r="D25">
-        <v>185</v>
+        <v>220</v>
       </c>
       <c r="E25">
-        <v>540000</v>
+        <v>1200000</v>
       </c>
       <c r="F25" s="1">
-        <v>45055.50114583333</v>
+        <v>45055.407534722224</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>4696508</v>
+        <v>4696481</v>
       </c>
       <c r="B26" t="s">
         <v>51</v>
@@ -1518,18 +1518,18 @@
         <v>52</v>
       </c>
       <c r="D26">
-        <v>220</v>
+        <v>170</v>
       </c>
       <c r="E26">
-        <v>1200000</v>
+        <v>480000</v>
       </c>
       <c r="F26" s="1">
-        <v>45055.407534722224</v>
+        <v>45055.40008101852</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>4696481</v>
+        <v>4696385</v>
       </c>
       <c r="B27" t="s">
         <v>53</v>
@@ -1538,18 +1538,18 @@
         <v>54</v>
       </c>
       <c r="D27">
-        <v>170</v>
+        <v>217</v>
       </c>
       <c r="E27">
-        <v>480000</v>
+        <v>2200000</v>
       </c>
       <c r="F27" s="1">
-        <v>45055.40008101852</v>
+        <v>45055.369791666664</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>4696385</v>
+        <v>4696376</v>
       </c>
       <c r="B28" t="s">
         <v>55</v>
@@ -1558,18 +1558,18 @@
         <v>56</v>
       </c>
       <c r="D28">
-        <v>217</v>
+        <v>88</v>
       </c>
       <c r="E28">
-        <v>2200000</v>
+        <v>600000</v>
       </c>
       <c r="F28" s="1">
-        <v>45055.369791666664</v>
+        <v>45055.365949074076</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>4696376</v>
+        <v>4696237</v>
       </c>
       <c r="B29" t="s">
         <v>57</v>
@@ -1578,18 +1578,18 @@
         <v>58</v>
       </c>
       <c r="D29">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="E29">
-        <v>600000</v>
+        <v>360000</v>
       </c>
       <c r="F29" s="1">
-        <v>45055.365949074076</v>
+        <v>45055.29398148148</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>4696237</v>
+        <v>4691228</v>
       </c>
       <c r="B30" t="s">
         <v>59</v>
@@ -1598,58 +1598,58 @@
         <v>60</v>
       </c>
       <c r="D30">
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="E30">
-        <v>360000</v>
+        <v>600000</v>
       </c>
       <c r="F30" s="1">
-        <v>45055.29398148148</v>
+        <v>45051.376435185186</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>4691228</v>
+        <v>4687890</v>
       </c>
       <c r="B31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" t="s">
         <v>61</v>
       </c>
-      <c r="C31" t="s">
-        <v>62</v>
-      </c>
       <c r="D31">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="E31">
-        <v>600000</v>
+        <v>1500000</v>
       </c>
       <c r="F31" s="1">
-        <v>45051.376435185186</v>
+        <v>45048.75144675926</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>4687890</v>
+        <v>4686980</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
         <v>63</v>
       </c>
       <c r="D32">
-        <v>120</v>
+        <v>161</v>
       </c>
       <c r="E32">
-        <v>1500000</v>
+        <v>1237186</v>
       </c>
       <c r="F32" s="1">
-        <v>45048.75144675926</v>
+        <v>45048.37636574074</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>4686980</v>
+        <v>4686827</v>
       </c>
       <c r="B33" t="s">
         <v>64</v>
@@ -1658,18 +1658,18 @@
         <v>65</v>
       </c>
       <c r="D33">
-        <v>161</v>
+        <v>54</v>
       </c>
       <c r="E33">
-        <v>1237186</v>
+        <v>95000</v>
       </c>
       <c r="F33" s="1">
-        <v>45048.37636574074</v>
+        <v>45048.295949074076</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>4686827</v>
+        <v>4684174</v>
       </c>
       <c r="B34" t="s">
         <v>66</v>
@@ -1678,18 +1678,18 @@
         <v>67</v>
       </c>
       <c r="D34">
-        <v>54</v>
+        <v>120</v>
       </c>
       <c r="E34">
-        <v>95000</v>
+        <v>1500000</v>
       </c>
       <c r="F34" s="1">
-        <v>45048.295949074076</v>
+        <v>45045.50996527778</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>4684174</v>
+        <v>4683331</v>
       </c>
       <c r="B35" t="s">
         <v>68</v>
@@ -1698,18 +1698,18 @@
         <v>69</v>
       </c>
       <c r="D35">
-        <v>120</v>
+        <v>149</v>
       </c>
       <c r="E35">
-        <v>1500000</v>
+        <v>2210200</v>
       </c>
       <c r="F35" s="1">
-        <v>45045.50996527778</v>
+        <v>45044.62634259259</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>4683331</v>
+        <v>4682762</v>
       </c>
       <c r="B36" t="s">
         <v>70</v>
@@ -1718,18 +1718,18 @@
         <v>71</v>
       </c>
       <c r="D36">
-        <v>149</v>
+        <v>241</v>
       </c>
       <c r="E36">
-        <v>2210200</v>
+        <v>565000</v>
       </c>
       <c r="F36" s="1">
-        <v>45044.62634259259</v>
+        <v>45044.375810185185</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>4682762</v>
+        <v>4679181</v>
       </c>
       <c r="B37" t="s">
         <v>72</v>
@@ -1738,18 +1738,18 @@
         <v>73</v>
       </c>
       <c r="D37">
-        <v>241</v>
+        <v>96</v>
       </c>
       <c r="E37">
-        <v>565000</v>
+        <v>1000000</v>
       </c>
       <c r="F37" s="1">
-        <v>45044.375810185185</v>
+        <v>45041.756875</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>4679181</v>
+        <v>4676005</v>
       </c>
       <c r="B38" t="s">
         <v>74</v>
@@ -1758,58 +1758,58 @@
         <v>75</v>
       </c>
       <c r="D38">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="E38">
-        <v>1000000</v>
+        <v>180000</v>
       </c>
       <c r="F38" s="1">
-        <v>45041.756875</v>
+        <v>45040.37637731482</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>4676005</v>
+        <v>4676002</v>
       </c>
       <c r="B39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" t="s">
         <v>76</v>
       </c>
-      <c r="C39" t="s">
-        <v>77</v>
-      </c>
       <c r="D39">
-        <v>55</v>
+        <v>160</v>
       </c>
       <c r="E39">
-        <v>180000</v>
+        <v>1009483</v>
       </c>
       <c r="F39" s="1">
-        <v>45040.37637731482</v>
+        <v>45040.37619212963</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>4676002</v>
+        <v>4673588</v>
       </c>
       <c r="B40" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="C40" t="s">
         <v>78</v>
       </c>
       <c r="D40">
-        <v>160</v>
+        <v>115</v>
       </c>
       <c r="E40">
-        <v>1009483</v>
+        <v>611000</v>
       </c>
       <c r="F40" s="1">
-        <v>45040.37619212963</v>
+        <v>45037.75806712963</v>
       </c>
     </row>
     <row r="41">
       <c r="A41">
-        <v>4673588</v>
+        <v>4672684</v>
       </c>
       <c r="B41" t="s">
         <v>79</v>
@@ -1818,18 +1818,18 @@
         <v>80</v>
       </c>
       <c r="D41">
-        <v>115</v>
+        <v>205</v>
       </c>
       <c r="E41">
-        <v>611000</v>
+        <v>1600000</v>
       </c>
       <c r="F41" s="1">
-        <v>45037.75806712963</v>
+        <v>45037.414189814815</v>
       </c>
     </row>
     <row r="42">
       <c r="A42">
-        <v>4672684</v>
+        <v>4668267</v>
       </c>
       <c r="B42" t="s">
         <v>81</v>
@@ -1838,18 +1838,18 @@
         <v>82</v>
       </c>
       <c r="D42">
-        <v>205</v>
+        <v>226</v>
       </c>
       <c r="E42">
-        <v>1600000</v>
+        <v>450000</v>
       </c>
       <c r="F42" s="1">
-        <v>45037.414189814815</v>
+        <v>45034.28559027778</v>
       </c>
     </row>
     <row r="43">
       <c r="A43">
-        <v>4668267</v>
+        <v>4664079</v>
       </c>
       <c r="B43" t="s">
         <v>83</v>
@@ -1858,18 +1858,18 @@
         <v>84</v>
       </c>
       <c r="D43">
-        <v>226</v>
+        <v>120</v>
       </c>
       <c r="E43">
-        <v>450000</v>
+        <v>360000</v>
       </c>
       <c r="F43" s="1">
-        <v>45034.28559027778</v>
+        <v>45029.50099537037</v>
       </c>
     </row>
     <row r="44">
       <c r="A44">
-        <v>4664079</v>
+        <v>4662382</v>
       </c>
       <c r="B44" t="s">
         <v>85</v>
@@ -1878,18 +1878,18 @@
         <v>86</v>
       </c>
       <c r="D44">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="E44">
         <v>360000</v>
       </c>
       <c r="F44" s="1">
-        <v>45029.50099537037</v>
+        <v>45028.376388888886</v>
       </c>
     </row>
     <row r="45">
       <c r="A45">
-        <v>4662382</v>
+        <v>4654221</v>
       </c>
       <c r="B45" t="s">
         <v>87</v>
@@ -1898,18 +1898,18 @@
         <v>88</v>
       </c>
       <c r="D45">
-        <v>94</v>
+        <v>241</v>
       </c>
       <c r="E45">
-        <v>360000</v>
+        <v>565000</v>
       </c>
       <c r="F45" s="1">
-        <v>45028.376388888886</v>
+        <v>45022.37645833333</v>
       </c>
     </row>
     <row r="46">
       <c r="A46">
-        <v>4654221</v>
+        <v>4652937</v>
       </c>
       <c r="B46" t="s">
         <v>89</v>
@@ -1924,12 +1924,12 @@
         <v>565000</v>
       </c>
       <c r="F46" s="1">
-        <v>45022.37645833333</v>
+        <v>45021.500972222224</v>
       </c>
     </row>
     <row r="47">
       <c r="A47">
-        <v>4652937</v>
+        <v>4644332</v>
       </c>
       <c r="B47" t="s">
         <v>91</v>
@@ -1938,18 +1938,18 @@
         <v>92</v>
       </c>
       <c r="D47">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="E47">
-        <v>565000</v>
+        <v>1517000</v>
       </c>
       <c r="F47" s="1">
-        <v>45021.500972222224</v>
+        <v>45015.38422453704</v>
       </c>
     </row>
     <row r="48">
       <c r="A48">
-        <v>4646972</v>
+        <v>4644331</v>
       </c>
       <c r="B48" t="s">
         <v>93</v>
@@ -1958,18 +1958,18 @@
         <v>94</v>
       </c>
       <c r="D48">
-        <v>80</v>
+        <v>226</v>
       </c>
       <c r="E48">
-        <v>210000</v>
+        <v>1532000</v>
       </c>
       <c r="F48" s="1">
-        <v>45016.7515625</v>
+        <v>45015.38422453704</v>
       </c>
     </row>
     <row r="49">
       <c r="A49">
-        <v>4644332</v>
+        <v>4644329</v>
       </c>
       <c r="B49" t="s">
         <v>95</v>
@@ -1978,18 +1978,18 @@
         <v>96</v>
       </c>
       <c r="D49">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E49">
-        <v>1517000</v>
+        <v>1215000</v>
       </c>
       <c r="F49" s="1">
-        <v>45015.38422453704</v>
+        <v>45015.384201388886</v>
       </c>
     </row>
     <row r="50">
       <c r="A50">
-        <v>4644331</v>
+        <v>4644328</v>
       </c>
       <c r="B50" t="s">
         <v>97</v>
@@ -1998,98 +1998,98 @@
         <v>98</v>
       </c>
       <c r="D50">
-        <v>226</v>
+        <v>114</v>
       </c>
       <c r="E50">
-        <v>1532000</v>
+        <v>611000</v>
       </c>
       <c r="F50" s="1">
-        <v>45015.38422453704</v>
+        <v>45015.384201388886</v>
       </c>
     </row>
     <row r="51">
       <c r="A51">
-        <v>4644329</v>
+        <v>4633169</v>
       </c>
       <c r="B51" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51" t="s">
         <v>99</v>
       </c>
-      <c r="C51" t="s">
-        <v>100</v>
-      </c>
       <c r="D51">
-        <v>227</v>
+        <v>206</v>
       </c>
       <c r="E51">
-        <v>1215000</v>
+        <v>1115000</v>
       </c>
       <c r="F51" s="1">
-        <v>45015.384201388886</v>
+        <v>45013.75430555556</v>
       </c>
     </row>
     <row r="52">
       <c r="A52">
-        <v>4644328</v>
+        <v>4633167</v>
       </c>
       <c r="B52" t="s">
-        <v>101</v>
+        <v>42</v>
       </c>
       <c r="C52" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D52">
-        <v>114</v>
+        <v>206</v>
       </c>
       <c r="E52">
-        <v>611000</v>
+        <v>920000</v>
       </c>
       <c r="F52" s="1">
-        <v>45015.384201388886</v>
+        <v>45013.754270833335</v>
       </c>
     </row>
     <row r="53">
       <c r="A53">
-        <v>4633169</v>
+        <v>4632180</v>
       </c>
       <c r="B53" t="s">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="C53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D53">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="E53">
-        <v>1115000</v>
+        <v>540000</v>
       </c>
       <c r="F53" s="1">
-        <v>45013.75430555556</v>
+        <v>45013.63730324074</v>
       </c>
     </row>
     <row r="54">
       <c r="A54">
-        <v>4633167</v>
+        <v>4617232</v>
       </c>
       <c r="B54" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="C54" t="s">
         <v>104</v>
       </c>
       <c r="D54">
-        <v>206</v>
+        <v>171</v>
       </c>
       <c r="E54">
-        <v>920000</v>
+        <v>2527435</v>
       </c>
       <c r="F54" s="1">
-        <v>45013.754270833335</v>
+        <v>45009.50215277778</v>
       </c>
     </row>
     <row r="55">
       <c r="A55">
-        <v>4632180</v>
+        <v>4617230</v>
       </c>
       <c r="B55" t="s">
         <v>105</v>
@@ -2098,18 +2098,18 @@
         <v>106</v>
       </c>
       <c r="D55">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="E55">
-        <v>540000</v>
+        <v>3188280</v>
       </c>
       <c r="F55" s="1">
-        <v>45013.63730324074</v>
+        <v>45009.502071759256</v>
       </c>
     </row>
     <row r="56">
       <c r="A56">
-        <v>4617232</v>
+        <v>4611644</v>
       </c>
       <c r="B56" t="s">
         <v>107</v>
@@ -2118,18 +2118,18 @@
         <v>108</v>
       </c>
       <c r="D56">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="E56">
-        <v>2527435</v>
+        <v>1047434</v>
       </c>
       <c r="F56" s="1">
-        <v>45009.50215277778</v>
+        <v>45008.37600694445</v>
       </c>
     </row>
     <row r="57">
       <c r="A57">
-        <v>4617230</v>
+        <v>4604346</v>
       </c>
       <c r="B57" t="s">
         <v>109</v>
@@ -2138,18 +2138,18 @@
         <v>110</v>
       </c>
       <c r="D57">
-        <v>204</v>
+        <v>86</v>
       </c>
       <c r="E57">
-        <v>3188280</v>
+        <v>2500000</v>
       </c>
       <c r="F57" s="1">
-        <v>45009.502071759256</v>
+        <v>45005.37855324074</v>
       </c>
     </row>
     <row r="58">
       <c r="A58">
-        <v>4611644</v>
+        <v>4601359</v>
       </c>
       <c r="B58" t="s">
         <v>111</v>
@@ -2158,18 +2158,18 @@
         <v>112</v>
       </c>
       <c r="D58">
-        <v>161</v>
+        <v>185</v>
       </c>
       <c r="E58">
-        <v>1047434</v>
+        <v>600000</v>
       </c>
       <c r="F58" s="1">
-        <v>45008.37600694445</v>
+        <v>45002.758472222224</v>
       </c>
     </row>
     <row r="59">
       <c r="A59">
-        <v>4604346</v>
+        <v>4591859</v>
       </c>
       <c r="B59" t="s">
         <v>113</v>
@@ -2178,18 +2178,18 @@
         <v>114</v>
       </c>
       <c r="D59">
-        <v>86</v>
+        <v>172</v>
       </c>
       <c r="E59">
-        <v>2500000</v>
+        <v>750000</v>
       </c>
       <c r="F59" s="1">
-        <v>45005.37855324074</v>
+        <v>45000.357881944445</v>
       </c>
     </row>
     <row r="60">
       <c r="A60">
-        <v>4601359</v>
+        <v>4591367</v>
       </c>
       <c r="B60" t="s">
         <v>115</v>
@@ -2198,18 +2198,18 @@
         <v>116</v>
       </c>
       <c r="D60">
-        <v>185</v>
+        <v>235</v>
       </c>
       <c r="E60">
-        <v>600000</v>
+        <v>2012000</v>
       </c>
       <c r="F60" s="1">
-        <v>45002.758472222224</v>
+        <v>44999.756898148145</v>
       </c>
     </row>
     <row r="61">
       <c r="A61">
-        <v>4591859</v>
+        <v>4582432</v>
       </c>
       <c r="B61" t="s">
         <v>117</v>
@@ -2218,18 +2218,18 @@
         <v>118</v>
       </c>
       <c r="D61">
-        <v>172</v>
+        <v>91</v>
       </c>
       <c r="E61">
-        <v>750000</v>
+        <v>360000</v>
       </c>
       <c r="F61" s="1">
-        <v>45000.357881944445</v>
+        <v>44994.38015046297</v>
       </c>
     </row>
     <row r="62">
       <c r="A62">
-        <v>4591367</v>
+        <v>4579437</v>
       </c>
       <c r="B62" t="s">
         <v>119</v>
@@ -2238,18 +2238,18 @@
         <v>120</v>
       </c>
       <c r="D62">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="E62">
-        <v>2012000</v>
+        <v>520000</v>
       </c>
       <c r="F62" s="1">
-        <v>44999.756898148145</v>
+        <v>44992.501493055555</v>
       </c>
     </row>
     <row r="63">
       <c r="A63">
-        <v>4582432</v>
+        <v>4559059</v>
       </c>
       <c r="B63" t="s">
         <v>121</v>
@@ -2258,18 +2258,18 @@
         <v>122</v>
       </c>
       <c r="D63">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="E63">
-        <v>360000</v>
+        <v>395000</v>
       </c>
       <c r="F63" s="1">
-        <v>44994.38015046297</v>
+        <v>44977.801782407405</v>
       </c>
     </row>
     <row r="64">
       <c r="A64">
-        <v>4579437</v>
+        <v>4558998</v>
       </c>
       <c r="B64" t="s">
         <v>123</v>
@@ -2278,18 +2278,18 @@
         <v>124</v>
       </c>
       <c r="D64">
-        <v>223</v>
+        <v>143</v>
       </c>
       <c r="E64">
-        <v>520000</v>
+        <v>495000</v>
       </c>
       <c r="F64" s="1">
-        <v>44992.501493055555</v>
+        <v>44977.76740740741</v>
       </c>
     </row>
     <row r="65">
       <c r="A65">
-        <v>4559059</v>
+        <v>4535313</v>
       </c>
       <c r="B65" t="s">
         <v>125</v>
@@ -2298,18 +2298,18 @@
         <v>126</v>
       </c>
       <c r="D65">
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="E65">
-        <v>395000</v>
+        <v>495000</v>
       </c>
       <c r="F65" s="1">
-        <v>44977.801782407405</v>
+        <v>44960.231261574074</v>
       </c>
     </row>
     <row r="66">
       <c r="A66">
-        <v>4558998</v>
+        <v>4524871</v>
       </c>
       <c r="B66" t="s">
         <v>127</v>
@@ -2318,18 +2318,18 @@
         <v>128</v>
       </c>
       <c r="D66">
-        <v>143</v>
+        <v>50</v>
       </c>
       <c r="E66">
-        <v>495000</v>
+        <v>110000</v>
       </c>
       <c r="F66" s="1">
-        <v>44977.76740740741</v>
+        <v>44952.604837962965</v>
       </c>
     </row>
     <row r="67">
       <c r="A67">
-        <v>4535313</v>
+        <v>4522275</v>
       </c>
       <c r="B67" t="s">
         <v>129</v>
@@ -2338,358 +2338,358 @@
         <v>130</v>
       </c>
       <c r="D67">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="E67">
-        <v>495000</v>
+        <v>2015000</v>
       </c>
       <c r="F67" s="1">
-        <v>44960.231261574074</v>
+        <v>44950.8783912037</v>
       </c>
     </row>
     <row r="68">
       <c r="A68">
-        <v>4524871</v>
+        <v>4521842</v>
       </c>
       <c r="B68" t="s">
+        <v>129</v>
+      </c>
+      <c r="C68" t="s">
         <v>131</v>
       </c>
-      <c r="C68" t="s">
-        <v>132</v>
-      </c>
       <c r="D68">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="E68">
-        <v>110000</v>
+        <v>607000</v>
       </c>
       <c r="F68" s="1">
-        <v>44952.604837962965</v>
+        <v>44950.769791666666</v>
       </c>
     </row>
     <row r="69">
       <c r="A69">
-        <v>4522275</v>
+        <v>4521833</v>
       </c>
       <c r="B69" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C69" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D69">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="E69">
-        <v>2015000</v>
+        <v>632000</v>
       </c>
       <c r="F69" s="1">
-        <v>44950.8783912037</v>
+        <v>44950.76898148148</v>
       </c>
     </row>
     <row r="70">
       <c r="A70">
-        <v>4521842</v>
+        <v>4521832</v>
       </c>
       <c r="B70" t="s">
+        <v>129</v>
+      </c>
+      <c r="C70" t="s">
         <v>133</v>
       </c>
-      <c r="C70" t="s">
-        <v>135</v>
-      </c>
       <c r="D70">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="E70">
-        <v>607000</v>
+        <v>688000</v>
       </c>
       <c r="F70" s="1">
-        <v>44950.769791666666</v>
+        <v>44950.76887731482</v>
       </c>
     </row>
     <row r="71">
       <c r="A71">
-        <v>4521833</v>
+        <v>4521826</v>
       </c>
       <c r="B71" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C71" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D71">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="E71">
-        <v>632000</v>
+        <v>698000</v>
       </c>
       <c r="F71" s="1">
-        <v>44950.76898148148</v>
+        <v>44950.76829861111</v>
       </c>
     </row>
     <row r="72">
       <c r="A72">
-        <v>4521832</v>
+        <v>4521821</v>
       </c>
       <c r="B72" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C72" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D72">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="E72">
-        <v>688000</v>
+        <v>622000</v>
       </c>
       <c r="F72" s="1">
-        <v>44950.76887731482</v>
+        <v>44950.7678125</v>
       </c>
     </row>
     <row r="73">
       <c r="A73">
-        <v>4521826</v>
+        <v>4521820</v>
       </c>
       <c r="B73" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C73" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D73">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="E73">
-        <v>698000</v>
+        <v>2016000</v>
       </c>
       <c r="F73" s="1">
-        <v>44950.76829861111</v>
+        <v>44950.767696759256</v>
       </c>
     </row>
     <row r="74">
       <c r="A74">
-        <v>4521821</v>
+        <v>4521817</v>
       </c>
       <c r="B74" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C74" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D74">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="E74">
-        <v>622000</v>
+        <v>1245000</v>
       </c>
       <c r="F74" s="1">
-        <v>44950.7678125</v>
+        <v>44950.7674537037</v>
       </c>
     </row>
     <row r="75">
       <c r="A75">
-        <v>4521820</v>
+        <v>4521808</v>
       </c>
       <c r="B75" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C75" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D75">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="E75">
-        <v>2016000</v>
+        <v>725000</v>
       </c>
       <c r="F75" s="1">
-        <v>44950.767696759256</v>
+        <v>44950.76645833333</v>
       </c>
     </row>
     <row r="76">
       <c r="A76">
-        <v>4521817</v>
+        <v>4521800</v>
       </c>
       <c r="B76" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C76" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D76">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E76">
-        <v>1245000</v>
+        <v>673000</v>
       </c>
       <c r="F76" s="1">
-        <v>44950.7674537037</v>
+        <v>44950.7659375</v>
       </c>
     </row>
     <row r="77">
       <c r="A77">
-        <v>4521808</v>
+        <v>4521781</v>
       </c>
       <c r="B77" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C77" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D77">
         <v>101</v>
       </c>
       <c r="E77">
-        <v>725000</v>
+        <v>735037</v>
       </c>
       <c r="F77" s="1">
-        <v>44950.76645833333</v>
+        <v>44950.76415509259</v>
       </c>
     </row>
     <row r="78">
       <c r="A78">
-        <v>4521800</v>
+        <v>4521774</v>
       </c>
       <c r="B78" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C78" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D78">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="E78">
-        <v>673000</v>
+        <v>1243000</v>
       </c>
       <c r="F78" s="1">
-        <v>44950.7659375</v>
+        <v>44950.76336805556</v>
       </c>
     </row>
     <row r="79">
       <c r="A79">
-        <v>4521781</v>
+        <v>4521767</v>
       </c>
       <c r="B79" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C79" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D79">
         <v>101</v>
       </c>
       <c r="E79">
-        <v>735037</v>
+        <v>710000</v>
       </c>
       <c r="F79" s="1">
-        <v>44950.76415509259</v>
+        <v>44950.762777777774</v>
       </c>
     </row>
     <row r="80">
       <c r="A80">
-        <v>4521774</v>
+        <v>4520216</v>
       </c>
       <c r="B80" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="C80" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D80">
-        <v>107</v>
+        <v>236</v>
       </c>
       <c r="E80">
-        <v>1243000</v>
+        <v>220000</v>
       </c>
       <c r="F80" s="1">
-        <v>44950.76336805556</v>
+        <v>44950.326840277776</v>
       </c>
     </row>
     <row r="81">
       <c r="A81">
-        <v>4521767</v>
+        <v>4516435</v>
       </c>
       <c r="B81" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="C81" t="s">
         <v>146</v>
       </c>
       <c r="D81">
-        <v>101</v>
+        <v>206</v>
       </c>
       <c r="E81">
-        <v>710000</v>
+        <v>2460000</v>
       </c>
       <c r="F81" s="1">
-        <v>44950.762777777774</v>
+        <v>44946.761608796296</v>
       </c>
     </row>
     <row r="82">
       <c r="A82">
-        <v>4520216</v>
+        <v>4516434</v>
       </c>
       <c r="B82" t="s">
+        <v>145</v>
+      </c>
+      <c r="C82" t="s">
         <v>147</v>
       </c>
-      <c r="C82" t="s">
-        <v>148</v>
-      </c>
       <c r="D82">
-        <v>236</v>
+        <v>206</v>
       </c>
       <c r="E82">
-        <v>220000</v>
+        <v>1410000</v>
       </c>
       <c r="F82" s="1">
-        <v>44950.326840277776</v>
+        <v>44946.7615625</v>
       </c>
     </row>
     <row r="83">
       <c r="A83">
-        <v>4516435</v>
+        <v>4516433</v>
       </c>
       <c r="B83" t="s">
+        <v>148</v>
+      </c>
+      <c r="C83" t="s">
         <v>149</v>
       </c>
-      <c r="C83" t="s">
-        <v>150</v>
-      </c>
       <c r="D83">
-        <v>206</v>
+        <v>173</v>
       </c>
       <c r="E83">
-        <v>2460000</v>
+        <v>1648000</v>
       </c>
       <c r="F83" s="1">
-        <v>44946.761608796296</v>
+        <v>44946.76150462963</v>
       </c>
     </row>
     <row r="84">
       <c r="A84">
-        <v>4516434</v>
+        <v>4516432</v>
       </c>
       <c r="B84" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C84" t="s">
         <v>151</v>
       </c>
       <c r="D84">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="E84">
-        <v>1410000</v>
+        <v>1660000</v>
       </c>
       <c r="F84" s="1">
-        <v>44946.7615625</v>
+        <v>44946.76144675926</v>
       </c>
     </row>
     <row r="85">
       <c r="A85">
-        <v>4516433</v>
+        <v>4514111</v>
       </c>
       <c r="B85" t="s">
         <v>152</v>
@@ -2698,18 +2698,18 @@
         <v>153</v>
       </c>
       <c r="D85">
-        <v>173</v>
+        <v>115</v>
       </c>
       <c r="E85">
-        <v>1648000</v>
+        <v>350000</v>
       </c>
       <c r="F85" s="1">
-        <v>44946.76150462963</v>
+        <v>44945.50115740741</v>
       </c>
     </row>
     <row r="86">
       <c r="A86">
-        <v>4516432</v>
+        <v>4506739</v>
       </c>
       <c r="B86" t="s">
         <v>154</v>
@@ -2718,78 +2718,78 @@
         <v>155</v>
       </c>
       <c r="D86">
-        <v>226</v>
+        <v>55</v>
       </c>
       <c r="E86">
-        <v>1660000</v>
+        <v>170000</v>
       </c>
       <c r="F86" s="1">
-        <v>44946.76144675926</v>
+        <v>44939.50289351852</v>
       </c>
     </row>
     <row r="87">
       <c r="A87">
-        <v>4514111</v>
+        <v>4499649</v>
       </c>
       <c r="B87" t="s">
+        <v>42</v>
+      </c>
+      <c r="C87" t="s">
         <v>156</v>
       </c>
-      <c r="C87" t="s">
-        <v>157</v>
-      </c>
       <c r="D87">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="E87">
-        <v>350000</v>
+        <v>698000</v>
       </c>
       <c r="F87" s="1">
-        <v>44945.50115740741</v>
+        <v>44933.751296296294</v>
       </c>
     </row>
     <row r="88">
       <c r="A88">
-        <v>4506739</v>
+        <v>4497393</v>
       </c>
       <c r="B88" t="s">
+        <v>157</v>
+      </c>
+      <c r="C88" t="s">
         <v>158</v>
       </c>
-      <c r="C88" t="s">
-        <v>159</v>
-      </c>
       <c r="D88">
-        <v>55</v>
+        <v>173</v>
       </c>
       <c r="E88">
-        <v>170000</v>
+        <v>1648000</v>
       </c>
       <c r="F88" s="1">
-        <v>44939.50289351852</v>
+        <v>44931.56686342593</v>
       </c>
     </row>
     <row r="89">
       <c r="A89">
-        <v>4499649</v>
+        <v>4497223</v>
       </c>
       <c r="B89" t="s">
-        <v>44</v>
+        <v>159</v>
       </c>
       <c r="C89" t="s">
         <v>160</v>
       </c>
       <c r="D89">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="E89">
-        <v>698000</v>
+        <v>345000</v>
       </c>
       <c r="F89" s="1">
-        <v>44933.751296296294</v>
+        <v>44931.50104166667</v>
       </c>
     </row>
     <row r="90">
       <c r="A90">
-        <v>4497393</v>
+        <v>4496890</v>
       </c>
       <c r="B90" t="s">
         <v>161</v>
@@ -2798,18 +2798,18 @@
         <v>162</v>
       </c>
       <c r="D90">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E90">
-        <v>1648000</v>
+        <v>600000</v>
       </c>
       <c r="F90" s="1">
-        <v>44931.56686342593</v>
+        <v>44931.35283564815</v>
       </c>
     </row>
     <row r="91">
       <c r="A91">
-        <v>4497223</v>
+        <v>4496881</v>
       </c>
       <c r="B91" t="s">
         <v>163</v>
@@ -2818,18 +2818,18 @@
         <v>164</v>
       </c>
       <c r="D91">
-        <v>98</v>
+        <v>153</v>
       </c>
       <c r="E91">
-        <v>345000</v>
+        <v>1100000</v>
       </c>
       <c r="F91" s="1">
-        <v>44931.50104166667</v>
+        <v>44931.34831018518</v>
       </c>
     </row>
     <row r="92">
       <c r="A92">
-        <v>4496890</v>
+        <v>4496874</v>
       </c>
       <c r="B92" t="s">
         <v>165</v>
@@ -2838,18 +2838,18 @@
         <v>166</v>
       </c>
       <c r="D92">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E92">
         <v>600000</v>
       </c>
       <c r="F92" s="1">
-        <v>44931.35283564815</v>
+        <v>44931.34423611111</v>
       </c>
     </row>
     <row r="93">
       <c r="A93">
-        <v>4496881</v>
+        <v>4488254</v>
       </c>
       <c r="B93" t="s">
         <v>167</v>
@@ -2858,18 +2858,18 @@
         <v>168</v>
       </c>
       <c r="D93">
-        <v>153</v>
+        <v>240</v>
       </c>
       <c r="E93">
-        <v>1100000</v>
+        <v>1539683</v>
       </c>
       <c r="F93" s="1">
-        <v>44931.34831018518</v>
+        <v>44922.62599537037</v>
       </c>
     </row>
     <row r="94">
       <c r="A94">
-        <v>4496874</v>
+        <v>4484881</v>
       </c>
       <c r="B94" t="s">
         <v>169</v>
@@ -2878,18 +2878,18 @@
         <v>170</v>
       </c>
       <c r="D94">
-        <v>173</v>
+        <v>210</v>
       </c>
       <c r="E94">
-        <v>600000</v>
+        <v>500000</v>
       </c>
       <c r="F94" s="1">
-        <v>44931.34423611111</v>
+        <v>44917.88123842593</v>
       </c>
     </row>
     <row r="95">
       <c r="A95">
-        <v>4488254</v>
+        <v>4434038</v>
       </c>
       <c r="B95" t="s">
         <v>171</v>
@@ -2898,18 +2898,18 @@
         <v>172</v>
       </c>
       <c r="D95">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="E95">
-        <v>1539683</v>
+        <v>1200000</v>
       </c>
       <c r="F95" s="1">
-        <v>44922.62599537037</v>
+        <v>44890.362222222226</v>
       </c>
     </row>
     <row r="96">
       <c r="A96">
-        <v>4484881</v>
+        <v>4429787</v>
       </c>
       <c r="B96" t="s">
         <v>173</v>
@@ -2918,98 +2918,98 @@
         <v>174</v>
       </c>
       <c r="D96">
-        <v>210</v>
+        <v>120</v>
       </c>
       <c r="E96">
-        <v>500000</v>
+        <v>70000</v>
       </c>
       <c r="F96" s="1">
-        <v>44917.88123842593</v>
+        <v>44888.7127662037</v>
       </c>
     </row>
     <row r="97">
       <c r="A97">
-        <v>4434038</v>
+        <v>4418604</v>
       </c>
       <c r="B97" t="s">
+        <v>159</v>
+      </c>
+      <c r="C97" t="s">
         <v>175</v>
       </c>
-      <c r="C97" t="s">
-        <v>176</v>
-      </c>
       <c r="D97">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="E97">
-        <v>1200000</v>
+        <v>320000</v>
       </c>
       <c r="F97" s="1">
-        <v>44890.362222222226</v>
+        <v>44880.50134259259</v>
       </c>
     </row>
     <row r="98">
       <c r="A98">
-        <v>4429787</v>
+        <v>4413895</v>
       </c>
       <c r="B98" t="s">
-        <v>177</v>
+        <v>115</v>
       </c>
       <c r="C98" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D98">
-        <v>120</v>
+        <v>237</v>
       </c>
       <c r="E98">
-        <v>70000</v>
+        <v>2020000</v>
       </c>
       <c r="F98" s="1">
-        <v>44888.7127662037</v>
+        <v>44876.37604166667</v>
       </c>
     </row>
     <row r="99">
       <c r="A99">
-        <v>4418604</v>
+        <v>4381872</v>
       </c>
       <c r="B99" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="C99" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D99">
-        <v>50</v>
+        <v>160</v>
       </c>
       <c r="E99">
-        <v>320000</v>
+        <v>1275137</v>
       </c>
       <c r="F99" s="1">
-        <v>44880.50134259259</v>
+        <v>44852.6440625</v>
       </c>
     </row>
     <row r="100">
       <c r="A100">
-        <v>4413895</v>
+        <v>4381871</v>
       </c>
       <c r="B100" t="s">
-        <v>119</v>
+        <v>179</v>
       </c>
       <c r="C100" t="s">
         <v>180</v>
       </c>
       <c r="D100">
-        <v>237</v>
+        <v>159</v>
       </c>
       <c r="E100">
-        <v>2020000</v>
+        <v>1001849</v>
       </c>
       <c r="F100" s="1">
-        <v>44876.37604166667</v>
+        <v>44852.6440162037</v>
       </c>
     </row>
     <row r="101">
       <c r="A101">
-        <v>4381872</v>
+        <v>4381322</v>
       </c>
       <c r="B101" t="s">
         <v>181</v>
@@ -3018,18 +3018,18 @@
         <v>182</v>
       </c>
       <c r="D101">
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="E101">
-        <v>1275137</v>
+        <v>380000</v>
       </c>
       <c r="F101" s="1">
-        <v>44852.6440625</v>
+        <v>44852.37667824074</v>
       </c>
     </row>
     <row r="102">
       <c r="A102">
-        <v>4381871</v>
+        <v>4373595</v>
       </c>
       <c r="B102" t="s">
         <v>183</v>
@@ -3038,18 +3038,18 @@
         <v>184</v>
       </c>
       <c r="D102">
-        <v>159</v>
+        <v>108</v>
       </c>
       <c r="E102">
-        <v>1001849</v>
+        <v>980000</v>
       </c>
       <c r="F102" s="1">
-        <v>44852.6440162037</v>
+        <v>44846.53739583334</v>
       </c>
     </row>
     <row r="103">
       <c r="A103">
-        <v>4381322</v>
+        <v>4373594</v>
       </c>
       <c r="B103" t="s">
         <v>185</v>
@@ -3058,18 +3058,18 @@
         <v>186</v>
       </c>
       <c r="D103">
-        <v>175</v>
+        <v>107</v>
       </c>
       <c r="E103">
-        <v>380000</v>
+        <v>1025000</v>
       </c>
       <c r="F103" s="1">
-        <v>44852.37667824074</v>
+        <v>44846.53738425926</v>
       </c>
     </row>
     <row r="104">
       <c r="A104">
-        <v>4373595</v>
+        <v>4373543</v>
       </c>
       <c r="B104" t="s">
         <v>187</v>
@@ -3078,18 +3078,18 @@
         <v>188</v>
       </c>
       <c r="D104">
-        <v>108</v>
+        <v>246</v>
       </c>
       <c r="E104">
-        <v>980000</v>
+        <v>1800000</v>
       </c>
       <c r="F104" s="1">
-        <v>44846.53739583334</v>
+        <v>44846.53538194444</v>
       </c>
     </row>
     <row r="105">
       <c r="A105">
-        <v>4373594</v>
+        <v>4372789</v>
       </c>
       <c r="B105" t="s">
         <v>189</v>
@@ -3098,18 +3098,18 @@
         <v>190</v>
       </c>
       <c r="D105">
-        <v>107</v>
+        <v>160</v>
       </c>
       <c r="E105">
-        <v>1025000</v>
+        <v>1000000</v>
       </c>
       <c r="F105" s="1">
-        <v>44846.53738425926</v>
+        <v>44846.38212962963</v>
       </c>
     </row>
     <row r="106">
       <c r="A106">
-        <v>4373543</v>
+        <v>4371249</v>
       </c>
       <c r="B106" t="s">
         <v>191</v>
@@ -3118,18 +3118,18 @@
         <v>192</v>
       </c>
       <c r="D106">
-        <v>246</v>
+        <v>216</v>
       </c>
       <c r="E106">
-        <v>1800000</v>
+        <v>1001849</v>
       </c>
       <c r="F106" s="1">
-        <v>44846.53538194444</v>
+        <v>44845.36756944445</v>
       </c>
     </row>
     <row r="107">
       <c r="A107">
-        <v>4372789</v>
+        <v>4371208</v>
       </c>
       <c r="B107" t="s">
         <v>193</v>
@@ -3138,18 +3138,18 @@
         <v>194</v>
       </c>
       <c r="D107">
-        <v>160</v>
+        <v>250</v>
       </c>
       <c r="E107">
-        <v>1000000</v>
+        <v>1200000</v>
       </c>
       <c r="F107" s="1">
-        <v>44846.38212962963</v>
+        <v>44845.363530092596</v>
       </c>
     </row>
     <row r="108">
       <c r="A108">
-        <v>4371249</v>
+        <v>4368905</v>
       </c>
       <c r="B108" t="s">
         <v>195</v>
@@ -3158,78 +3158,78 @@
         <v>196</v>
       </c>
       <c r="D108">
-        <v>216</v>
+        <v>94</v>
       </c>
       <c r="E108">
-        <v>1001849</v>
+        <v>805000</v>
       </c>
       <c r="F108" s="1">
-        <v>44845.36756944445</v>
+        <v>44844.39549768518</v>
       </c>
     </row>
     <row r="109">
       <c r="A109">
-        <v>4371208</v>
+        <v>4320354</v>
       </c>
       <c r="B109" t="s">
+        <v>159</v>
+      </c>
+      <c r="C109" t="s">
         <v>197</v>
       </c>
-      <c r="C109" t="s">
-        <v>198</v>
-      </c>
       <c r="D109">
-        <v>250</v>
+        <v>128</v>
       </c>
       <c r="E109">
-        <v>1200000</v>
+        <v>340000</v>
       </c>
       <c r="F109" s="1">
-        <v>44845.363530092596</v>
+        <v>44809.51527777778</v>
       </c>
     </row>
     <row r="110">
       <c r="A110">
-        <v>4368905</v>
+        <v>4320275</v>
       </c>
       <c r="B110" t="s">
+        <v>198</v>
+      </c>
+      <c r="C110" t="s">
         <v>199</v>
       </c>
-      <c r="C110" t="s">
-        <v>200</v>
-      </c>
       <c r="D110">
-        <v>94</v>
+        <v>175</v>
       </c>
       <c r="E110">
-        <v>805000</v>
+        <v>380000</v>
       </c>
       <c r="F110" s="1">
-        <v>44844.39549768518</v>
+        <v>44809.50917824074</v>
       </c>
     </row>
     <row r="111">
       <c r="A111">
-        <v>4320354</v>
+        <v>4320244</v>
       </c>
       <c r="B111" t="s">
-        <v>163</v>
+        <v>200</v>
       </c>
       <c r="C111" t="s">
         <v>201</v>
       </c>
       <c r="D111">
-        <v>128</v>
+        <v>153</v>
       </c>
       <c r="E111">
-        <v>340000</v>
+        <v>1100000</v>
       </c>
       <c r="F111" s="1">
-        <v>44809.51527777778</v>
+        <v>44809.507372685184</v>
       </c>
     </row>
     <row r="112">
       <c r="A112">
-        <v>4320275</v>
+        <v>4320241</v>
       </c>
       <c r="B112" t="s">
         <v>202</v>
@@ -3238,238 +3238,238 @@
         <v>203</v>
       </c>
       <c r="D112">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E112">
-        <v>380000</v>
+        <v>790000</v>
       </c>
       <c r="F112" s="1">
-        <v>44809.50917824074</v>
+        <v>44809.50716435185</v>
       </c>
     </row>
     <row r="113">
       <c r="A113">
-        <v>4320244</v>
+        <v>4320234</v>
       </c>
       <c r="B113" t="s">
+        <v>59</v>
+      </c>
+      <c r="C113" t="s">
         <v>204</v>
       </c>
-      <c r="C113" t="s">
-        <v>205</v>
-      </c>
       <c r="D113">
-        <v>153</v>
+        <v>80</v>
       </c>
       <c r="E113">
-        <v>1100000</v>
+        <v>558000</v>
       </c>
       <c r="F113" s="1">
-        <v>44809.507372685184</v>
+        <v>44809.506261574075</v>
       </c>
     </row>
     <row r="114">
       <c r="A114">
-        <v>4320241</v>
+        <v>4320208</v>
       </c>
       <c r="B114" t="s">
+        <v>205</v>
+      </c>
+      <c r="C114" t="s">
         <v>206</v>
       </c>
-      <c r="C114" t="s">
-        <v>207</v>
-      </c>
       <c r="D114">
-        <v>173</v>
+        <v>137</v>
       </c>
       <c r="E114">
-        <v>790000</v>
+        <v>684000</v>
       </c>
       <c r="F114" s="1">
-        <v>44809.50716435185</v>
+        <v>44809.50413194444</v>
       </c>
     </row>
     <row r="115">
       <c r="A115">
-        <v>4320234</v>
+        <v>4320206</v>
       </c>
       <c r="B115" t="s">
-        <v>61</v>
+        <v>205</v>
       </c>
       <c r="C115" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D115">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="E115">
-        <v>558000</v>
+        <v>270000</v>
       </c>
       <c r="F115" s="1">
-        <v>44809.506261574075</v>
+        <v>44809.504108796296</v>
       </c>
     </row>
     <row r="116">
       <c r="A116">
-        <v>4320208</v>
+        <v>4320205</v>
       </c>
       <c r="B116" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C116" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D116">
-        <v>137</v>
+        <v>165</v>
       </c>
       <c r="E116">
-        <v>684000</v>
+        <v>1613000</v>
       </c>
       <c r="F116" s="1">
-        <v>44809.50413194444</v>
+        <v>44809.50409722222</v>
       </c>
     </row>
     <row r="117">
       <c r="A117">
-        <v>4320206</v>
+        <v>4320181</v>
       </c>
       <c r="B117" t="s">
         <v>209</v>
       </c>
       <c r="C117" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D117">
-        <v>108</v>
+        <v>176</v>
       </c>
       <c r="E117">
-        <v>270000</v>
+        <v>1350000</v>
       </c>
       <c r="F117" s="1">
-        <v>44809.504108796296</v>
+        <v>44809.50266203703</v>
       </c>
     </row>
     <row r="118">
       <c r="A118">
-        <v>4320205</v>
+        <v>4319975</v>
       </c>
       <c r="B118" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C118" t="s">
         <v>212</v>
       </c>
       <c r="D118">
-        <v>165</v>
+        <v>198</v>
       </c>
       <c r="E118">
-        <v>1613000</v>
+        <v>875000</v>
       </c>
       <c r="F118" s="1">
-        <v>44809.50409722222</v>
+        <v>44809.382685185185</v>
       </c>
     </row>
     <row r="119">
       <c r="A119">
-        <v>4320181</v>
+        <v>4319904</v>
       </c>
       <c r="B119" t="s">
+        <v>159</v>
+      </c>
+      <c r="C119" t="s">
         <v>213</v>
       </c>
-      <c r="C119" t="s">
-        <v>214</v>
-      </c>
       <c r="D119">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="E119">
-        <v>1350000</v>
+        <v>600000</v>
       </c>
       <c r="F119" s="1">
-        <v>44809.50266203703</v>
+        <v>44809.376875</v>
       </c>
     </row>
     <row r="120">
       <c r="A120">
-        <v>4319975</v>
+        <v>4289884</v>
       </c>
       <c r="B120" t="s">
+        <v>214</v>
+      </c>
+      <c r="C120" t="s">
         <v>215</v>
       </c>
-      <c r="C120" t="s">
-        <v>216</v>
-      </c>
       <c r="D120">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="E120">
-        <v>875000</v>
+        <v>240000</v>
       </c>
       <c r="F120" s="1">
-        <v>44809.382685185185</v>
+        <v>44784.44188657407</v>
       </c>
     </row>
     <row r="121">
       <c r="A121">
-        <v>4319904</v>
+        <v>4243364</v>
       </c>
       <c r="B121" t="s">
-        <v>163</v>
+        <v>72</v>
       </c>
       <c r="C121" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D121">
-        <v>185</v>
+        <v>96</v>
       </c>
       <c r="E121">
-        <v>600000</v>
+        <v>1000000</v>
       </c>
       <c r="F121" s="1">
-        <v>44809.376875</v>
+        <v>44750.76640046296</v>
       </c>
     </row>
     <row r="122">
       <c r="A122">
-        <v>4289884</v>
+        <v>4238463</v>
       </c>
       <c r="B122" t="s">
+        <v>217</v>
+      </c>
+      <c r="C122" t="s">
         <v>218</v>
       </c>
-      <c r="C122" t="s">
-        <v>219</v>
-      </c>
       <c r="D122">
-        <v>180</v>
+        <v>230</v>
       </c>
       <c r="E122">
-        <v>240000</v>
+        <v>100000</v>
       </c>
       <c r="F122" s="1">
-        <v>44784.44188657407</v>
+        <v>44747.54550925926</v>
       </c>
     </row>
     <row r="123">
       <c r="A123">
-        <v>4243364</v>
+        <v>4232186</v>
       </c>
       <c r="B123" t="s">
-        <v>74</v>
+        <v>219</v>
       </c>
       <c r="C123" t="s">
         <v>220</v>
       </c>
       <c r="D123">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="E123">
-        <v>1000000</v>
+        <v>275000</v>
       </c>
       <c r="F123" s="1">
-        <v>44750.76640046296</v>
+        <v>44743.36004629629</v>
       </c>
     </row>
     <row r="124">
       <c r="A124">
-        <v>4238463</v>
+        <v>4169238</v>
       </c>
       <c r="B124" t="s">
         <v>221</v>
@@ -3478,18 +3478,18 @@
         <v>222</v>
       </c>
       <c r="D124">
-        <v>230</v>
+        <v>246</v>
       </c>
       <c r="E124">
-        <v>100000</v>
+        <v>1750000</v>
       </c>
       <c r="F124" s="1">
-        <v>44747.54550925926</v>
+        <v>44694.63559027778</v>
       </c>
     </row>
     <row r="125">
       <c r="A125">
-        <v>4232186</v>
+        <v>4088917</v>
       </c>
       <c r="B125" t="s">
         <v>223</v>
@@ -3498,18 +3498,18 @@
         <v>224</v>
       </c>
       <c r="D125">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="E125">
-        <v>275000</v>
+        <v>345000</v>
       </c>
       <c r="F125" s="1">
-        <v>44743.36004629629</v>
+        <v>44641.631574074076</v>
       </c>
     </row>
     <row r="126">
       <c r="A126">
-        <v>4169238</v>
+        <v>3868167</v>
       </c>
       <c r="B126" t="s">
         <v>225</v>
@@ -3518,13 +3518,13 @@
         <v>226</v>
       </c>
       <c r="D126">
-        <v>246</v>
+        <v>71</v>
       </c>
       <c r="E126">
-        <v>1750000</v>
+        <v>520000</v>
       </c>
       <c r="F126" s="1">
-        <v>44694.63559027778</v>
+        <v>44490.56721064815</v>
       </c>
     </row>
   </sheetData>

</xml_diff>